<commit_message>
calculate again and correct error
</commit_message>
<xml_diff>
--- a/tree.xlsx
+++ b/tree.xlsx
@@ -57395,7 +57395,7 @@
         <v>0</v>
       </c>
       <c r="AC612" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="613">
@@ -71066,7 +71066,7 @@
         <v>919.3200000000001</v>
       </c>
       <c r="AC759" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="760">

</xml_diff>